<commit_message>
Updated 12 indicator LSTM to have 200 epoch
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -64,7 +64,7 @@
     <t>﻿0.975178</t>
   </si>
   <si>
-    <t>LSTM with first 8 indicators, 100 units, 5 cells)</t>
+    <t>LSTM with first 8 indicators, 100 units, 5 cells, 60 timesteps)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:E420"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
LSTM with 75 time steps
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="15">
   <si>
     <t>_0.975178</t>
   </si>
@@ -351,6 +351,3406 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AX$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.9419769</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AX$7:$AX$421</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="415"/>
+                <c:pt idx="0">
+                  <c:v>0.94627315</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9487417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9504345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9523371</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9552573</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95993906</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.964939</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96974623</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.973526</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9757819</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9785183</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9810343</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.98315793</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98429215</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.9847945</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.98561186</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.98565465</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9840155</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.98292756</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97788167</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9742574</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96899706</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.96587825</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.96472824</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.96392137</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.9640859</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.96488893</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.9643039</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.9648252</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.965232</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.96737957</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.96883166</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.9666264</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.96349066</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96265626</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.96349955</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.9644841</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.9640503</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.964328</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.96444064</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.96575123</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.967164</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.9683615</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.97211206</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.9752132</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.97726315</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.97912544</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.98077154</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.9790574</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9783918</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.9793805</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.9809761</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.9835226</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.9869726</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.98879194</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.98884785</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.988164</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.98442125</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.98270667</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.9848841</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.9848939</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.9823121</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.9802548</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.9810834</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.9838015</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.98437274</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.98476654</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.98601</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.9889842</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.99193215</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.9937741</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.99422807</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.9945617</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.99526197</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.99289054</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.9909104</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.99049276</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.98929316</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.98839056</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.98737687</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.98778224</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.98613256</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.98371655</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.9812955</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.97955215</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.9792042</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.9816291</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.9826159</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.98083913</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.97952676</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.9792551</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.98043674</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.9814288</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.982596</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.9843919</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.9845849</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.98364097</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.9813999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.9747928</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.96907234</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.96658736</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.967406</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.96805507</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.96647406</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.96331364</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.9605037</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.95925105</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.96074086</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.96468806</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.9687892</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.9726756</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.97625464</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.9790211</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.98044235</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.98121905</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.9807993</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.97898525</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.9772287</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.9761419</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.9773247</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.9793313</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.98132616</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.9816593</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.98109114</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.98031056</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.9777444</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.9752131</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.9749125</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.9748626</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.9732658</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.9735342</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.9750629</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.9766014</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.97876346</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.9774776</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.9706349</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.9588715</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.9428812</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.9284641</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.91873544</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.9159695</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.919169</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.92279845</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.920304</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.9166465</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.9137817</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.91034514</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.9075248</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.9059042</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.90796167</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.91365284</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.9200865</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.92533743</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.9303282</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.9337146</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.93311197</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.9329148</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.93074805</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.9296675</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.92783195</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.92686707</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.9231523</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.91996324</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.9185138</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.91905594</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.9187694</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.9209801</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.9256231</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.9304896</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.9349553</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.9399548</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.9449621</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.94815266</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.9500065</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.9512857</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.9540765</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.95788187</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.9616271</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.9636692</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.96488136</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.9672686</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.9704418</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.97212255</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.9722776</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.97358155</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.9747077</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.9756777</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.97708875</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.9783352</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.97905415</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.9791842</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.9774141</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.97578746</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.974685</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.9708578</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.9650615</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.96057105</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.95921755</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.9595185</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.962095</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.9645013</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.9659609</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.9654722</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.96607816</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.96758854</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.9675303</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.96774566</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.9669212</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.96297216</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.9599188</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.95862544</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.9563353</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.9521925</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.95031935</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.9466234</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.9433152</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.94238895</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.9439368</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.9449831</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.94193494</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.94038534</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.9410651</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.9438399</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.94938594</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.9538595</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.9576805</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.96071213</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.96128124</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.9557523</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.9510314</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.94606924</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.9395788</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.9335243</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.9289307</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.9262518</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.92138994</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.9162113</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.9095961</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.9044357</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.89737475</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.8922683</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.8903151</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.890552</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.8929001</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.8943099</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.89574116</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.8980602</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.90274656</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.90529203</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.9055612</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.9071888</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.9069039</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.9029081</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.8987881</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.8969362</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.8944139</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.8940203</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.8966835</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.9012337</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.9067033</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>0.91141254</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.91561294</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0.91807365</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.9180656</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>0.91960835</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.92264843</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>0.92480576</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>0.92650175</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>0.93091315</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.936058</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.93951815</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>0.9422665</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>0.9431468</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>0.94410104</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>0.9439056</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>0.94521046</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>0.9487355</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.95221317</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.95518154</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.9573399</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>0.9589545</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.9607497</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>0.96168214</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.96142966</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>0.9607245</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>0.9609335</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>0.9610915</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>0.96291506</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>0.96488285</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>0.96518403</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>0.9659981</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>0.96374154</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>0.96154755</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>0.9574059</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>0.95492303</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>0.95366675</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>0.9537606</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.95657504</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>0.96073115</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>0.9637139</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>0.96506</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>0.96614224</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>0.9663445</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>0.9654738</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>0.9641996</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>0.9636093</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>0.9645029</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>0.96582663</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>0.96506464</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>0.9613564</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>0.959348</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>0.95675546</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>0.95425373</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>0.9528324</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>0.9523709</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>0.9535475</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>0.9553388</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>0.95626056</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>0.9554818</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>0.9525302</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>0.9501831</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>0.94717395</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>0.94393677</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>0.9410325</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>0.9413116</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>0.9440146</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>0.9475004</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>0.9525916</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>0.95750284</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>0.96126217</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>0.9625025</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>0.9628873</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>0.9635621</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>0.96465504</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>0.9671925</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>0.97097206</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>0.9754118</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>0.9791957</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>0.97952676</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>0.9771114</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>0.9729521</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>0.97011</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>0.96781945</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>0.9670979</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>0.96794534</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>0.97082967</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>0.9733941</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>0.9754484</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>0.96660954</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>0.95389414</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>0.9450285</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>0.94309694</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>0.94683295</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>0.95415556</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>0.9592503</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>0.9614791</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>0.96261615</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>0.96381307</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>0.9670429</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>0.97064656</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>0.97509986</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>0.97972435</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>0.9840811</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>0.98828065</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>0.9918199</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>0.99486715</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>0.9970552</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>0.99956477</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>1.0018375</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>1.0034516</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>1.0041698</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>1.0047411</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>1.006051</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>1.0077393</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>1.0045644</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>1.001814</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>1.001192</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>1.0044937</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>1.008986</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>1.0119861</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>1.0123028</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>1.0120353</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>1.0119597</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>1.0124478</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>1.0118601</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>1.0106826</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>1.0113138</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>1.0118636</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>1.0126</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>1.0143278</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>1.0125443</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>1.0094018</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>1.0054506</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>1.0047951</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>1.0052414</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>1.0039638</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>1.002387</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>1.0035387</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>1.0061804</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>1.0086383</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>1.0094285</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>1.0005858</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>0.9917021</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>0.9846392</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>0.98178124</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>0.98186773</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>0.98264027</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>0.98386085</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>0.9850419</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>0.9859715</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>0.98783976</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>0.9893356</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>0.9885133</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>0.9877014</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>0.9884188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AY$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>﻿0.975178</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AY$7:$AY$421</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="415"/>
+                <c:pt idx="0">
+                  <c:v>0.969004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.984456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.984413</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.998522</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.00454</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.00691</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.00644</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.00487</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.01395</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0135</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.01762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.01647</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.01426</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.00985</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.01897</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.01217</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.00563</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0074</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.986344</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.992122</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.967179</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.964407</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.982589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.973714</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.993367</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98848</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.00632</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.999081</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0124</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.00979</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.00066</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.979124</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.975658</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.979102</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.996938</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.983961</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.978162</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.983303</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.992963</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.98993</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.993869</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.00043</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.00813</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.00132</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.00373</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.01136</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0102</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.993359</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.00695</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.00475</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.0123</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.01581</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.01918</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.01298</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.01711</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.01151</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.996422</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.01253</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.01692</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.999215</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.992631</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.998183</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.01805</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.01044</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.00605</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.00559</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.02159</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.02274</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.02732</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.02635</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.02495</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.02846</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.0251</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.00964</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.02327</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.02137</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.01189</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.01496</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.01346</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.01662</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.00373</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.0016</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.992016</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.992631</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.01035</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.01293</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.0025</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.995658</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.00405</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.00698</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.02169</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.01373</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.02283</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.02378</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.01274</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.0083</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.00772</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.976712</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98058</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.9907</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.990248</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.984576</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.993473</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.968961</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.972236</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.990135</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.00639</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.013</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.0119</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.02385</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.02551</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.02667</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.02025</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.01668</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.00819</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.992277</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.983784</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.0019</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.01273</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.01277</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.00938</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.00528</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.00194</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.00656</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.995043</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.990806</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.00962</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.995403</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.996803</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.994922</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.00069</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1.00839</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1.00449</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.992249</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.961218</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.915363</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.860428</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.842324</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.893879</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.927223</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.928078</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.916275</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.875025</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.899784</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.901389</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.880237</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.914316</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.894961</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.902209</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.908404</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.902733</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.920455</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.932633</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.929019</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.906269</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.912591</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.895456</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.892641</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.88803</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.887394</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.852338</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.853979</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.879395</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.882075</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.901552</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.926791</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.921749</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.933</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.945447</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.94648</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.948297</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.938559</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.931876</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.952823</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.959365</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.959754</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.95771</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.949344</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.973084</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.989095</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.986288</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.982546</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.999844</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.99918</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.992072</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1.00953</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1.01359</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1.0083</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1.00662</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1.0061</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.991521</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.993741</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.988989</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.968459</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.952243</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.973565</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.97162</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.995057</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.993402</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.99901</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.997185</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.998989</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.998798</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.999675</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.992815</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1.00853</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.992178</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.97104</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1.00079</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.990453</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.98092</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.969626</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.972886</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.944697</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.951465</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.966649</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.987624</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.965574</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.939874</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.950907</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.963509</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.981415</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.979081</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.975906</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.991365</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.980757</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.967024</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.944903</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.947767</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.929061</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.895703</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.88081</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.881969</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.892584</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.858356</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.880675</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.85132</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.852027</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.836469</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.8433</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.87011</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>0.849021</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.867797</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>0.853172</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.860534</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.893688</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>0.893079</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>0.867373</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.874091</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>0.876156</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>0.851122</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>0.832303</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>0.831433</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>0.831186</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>0.815076</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>0.840323</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>0.862104</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>0.884197</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>0.877839</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>0.877804</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>0.897407</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>0.880272</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>0.886304</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>0.901792</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>0.899211</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>0.888023</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>0.920639</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>0.926367</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>0.931282</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>0.935942</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>0.937194</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>0.921282</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>0.928354</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>0.928573</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>0.951642</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>0.949839</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>0.947215</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>0.955199</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>0.964654</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>0.971012</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>0.972441</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>0.971168</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>0.961911</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>0.961366</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>0.962151</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>0.974852</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>0.981175</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>0.978197</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>0.987419</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>0.982716</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>0.967893</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>0.983091</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>0.965588</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>0.969612</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>0.965645</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>0.979597</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>0.994236</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.994491</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>0.993041</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>1.00267</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>1.00723</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>1.00837</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>1.00064</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>1.00071</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>0.998034</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>1.0008</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>1.00324</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>0.989562</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>0.982129</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>0.993536</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>0.980764</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>0.972101</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>0.971755</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>0.976359</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>0.977455</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>0.99563</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>0.981535</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>0.981288</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>0.968912</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>0.983091</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>0.969336</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>0.969633</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>0.964266</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>0.97295</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>0.969923</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>0.989739</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>0.999979</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>0.999668</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1.006</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1.00452</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>1.0062</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>1.01039</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1.00605</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>1.01332</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>1.01525</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>1.02019</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>1.01762</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>1.00389</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>0.99186</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>0.989215</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>0.986514</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>0.991104</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>0.986316</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>0.994823</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>0.998819</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>0.996379</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>1.01609</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>0.962406</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>0.936331</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>0.961472</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>0.985998</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>1.00586</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>1.00876</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>0.998571</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>1.00648</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>1.00518</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>1.02781</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>1.03295</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>1.04354</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>1.04375</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>1.05175</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>1.05033</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>1.05397</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>1.05177</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>1.05831</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>1.05276</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>1.05973</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>1.0551</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>1.05559</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>1.05375</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>1.05621</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>1.05872</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>1.05677</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>1.047</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>1.05178</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>1.05211</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>1.06527</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>1.06387</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>1.06447</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>1.06005</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>1.06734</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>1.06611</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>1.07042</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>1.06194</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>1.06481</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>1.06821</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>1.06598</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>1.06511</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>1.06812</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>1.06002</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>1.05792</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>1.05549</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>1.06351</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>1.0605</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>1.05684</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>1.05678</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>1.06323</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>1.06783</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>1.0676</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>1.06416</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>1.02634</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>1.04842</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>1.02578</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>1.02489</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>1.04009</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>1.03436</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>1.03433</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>1.03479</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>1.05131</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>1.06125</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>1.05242</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>1.03927</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>1.04905</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>1.05714</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>1.04283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1926066624"/>
+        <c:axId val="-1925783232"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1926066624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1925783232"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1925783232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1926066624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -614,10 +4014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC422"/>
+  <dimension ref="A1:BJ422"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" topLeftCell="AP2" workbookViewId="0">
+      <selection activeCell="BH24" sqref="BH24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +4035,7 @@
     <col min="40" max="40" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -780,8 +4180,26 @@
       <c r="BC1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="BE1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>6</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>7</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -926,12 +4344,30 @@
       <c r="BC2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="BE2">
+        <v>100</v>
+      </c>
+      <c r="BF2">
+        <v>60</v>
+      </c>
+      <c r="BG2">
+        <v>5</v>
+      </c>
+      <c r="BH2">
+        <v>200</v>
+      </c>
+      <c r="BI2">
+        <v>16</v>
+      </c>
+      <c r="BJ2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="AF3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -987,7 +4423,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.97099155000000004</v>
       </c>
@@ -1075,7 +4511,7 @@
         <v>0.9115949734007408</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.97150199999999998</v>
       </c>
@@ -1129,7 +4565,7 @@
         <v>0.96900399999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.97180370000000005</v>
       </c>
@@ -1179,7 +4615,7 @@
         <v>0.984456</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.97260636</v>
       </c>
@@ -1229,7 +4665,7 @@
         <v>0.98441299999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.97358080000000002</v>
       </c>
@@ -1279,7 +4715,7 @@
         <v>0.99852200000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.97455656999999996</v>
       </c>
@@ -1329,7 +4765,7 @@
         <v>1.00454</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.97525066000000005</v>
       </c>
@@ -1379,7 +4815,7 @@
         <v>1.00691</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.97576589999999996</v>
       </c>
@@ -1429,7 +4865,7 @@
         <v>1.00644</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.97638970000000003</v>
       </c>
@@ -1479,7 +4915,7 @@
         <v>1.0048699999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.97705995999999995</v>
       </c>
@@ -1529,7 +4965,7 @@
         <v>1.0139499999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.97779329999999998</v>
       </c>
@@ -21837,6 +25273,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SAE output round 2
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="21">
   <si>
     <t>_0.975178</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>(Sliding window)</t>
+  </si>
+  <si>
+    <t>SAE output without closing price</t>
+  </si>
+  <si>
+    <t>SAE output with closing price</t>
   </si>
 </sst>
 </file>
@@ -10811,10 +10817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DN422"/>
+  <dimension ref="A1:EB422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX1" zoomScaleNormal="283" workbookViewId="0">
-      <selection activeCell="DM20" sqref="DM20"/>
+    <sheetView tabSelected="1" topLeftCell="DL1" zoomScaleNormal="283" workbookViewId="0">
+      <selection activeCell="DX14" sqref="DX14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10832,7 +10838,7 @@
     <col min="40" max="40" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -11139,8 +11145,44 @@
       <c r="DN1" t="s">
         <v>9</v>
       </c>
+      <c r="DP1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>4</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>5</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>6</v>
+      </c>
+      <c r="DT1" t="s">
+        <v>7</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>9</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>4</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>5</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>6</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>7</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -11447,8 +11489,44 @@
       <c r="DN2">
         <v>90</v>
       </c>
+      <c r="DP2">
+        <v>100</v>
+      </c>
+      <c r="DQ2">
+        <v>60</v>
+      </c>
+      <c r="DR2">
+        <v>5</v>
+      </c>
+      <c r="DS2">
+        <v>250</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>19</v>
+      </c>
+      <c r="DU2">
+        <v>90</v>
+      </c>
+      <c r="DW2">
+        <v>100</v>
+      </c>
+      <c r="DX2">
+        <v>60</v>
+      </c>
+      <c r="DY2">
+        <v>5</v>
+      </c>
+      <c r="DZ2">
+        <v>250</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>20</v>
+      </c>
+      <c r="EB2">
+        <v>90</v>
+      </c>
     </row>
-    <row r="3" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:132" x14ac:dyDescent="0.2">
       <c r="AF3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="CN3" t="s">
@@ -11461,7 +11539,7 @@
         <v>0.94888378097442105</v>
       </c>
     </row>
-    <row r="4" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:132" x14ac:dyDescent="0.2">
       <c r="CG4">
         <v>0</v>
       </c>
@@ -11480,8 +11558,11 @@
       <c r="DI4">
         <v>0.81526411186815295</v>
       </c>
+      <c r="DP4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -11599,8 +11680,11 @@
         <f>AVERAGE(DI3:DI14)</f>
         <v>0.78156800969451756</v>
       </c>
+      <c r="DP5">
+        <v>0.95472717442714194</v>
+      </c>
     </row>
-    <row r="6" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.97099155000000004</v>
       </c>
@@ -11751,8 +11835,11 @@
       <c r="DI6">
         <v>0.85343773138027901</v>
       </c>
+      <c r="DP6">
+        <v>0.83085067572085103</v>
+      </c>
     </row>
-    <row r="7" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.97150199999999998</v>
       </c>
@@ -11853,8 +11940,15 @@
       <c r="DI7">
         <v>0.923413939018916</v>
       </c>
+      <c r="DP7">
+        <v>0.93072949372316804</v>
+      </c>
+      <c r="DQ7">
+        <f>AVERAGE(DP5:DP16)</f>
+        <v>0.75696277223899677</v>
+      </c>
     </row>
-    <row r="8" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.97180370000000005</v>
       </c>
@@ -11959,8 +12053,11 @@
       <c r="DI8">
         <v>0.70215514627930098</v>
       </c>
+      <c r="DP8">
+        <v>0.85948894263700704</v>
+      </c>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.97260636</v>
       </c>
@@ -12057,8 +12154,11 @@
       <c r="DI9">
         <v>0.863487205803802</v>
       </c>
+      <c r="DP9">
+        <v>0.91203822396899004</v>
+      </c>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.97358080000000002</v>
       </c>
@@ -12155,8 +12255,11 @@
       <c r="DI10">
         <v>0.89147153010811597</v>
       </c>
+      <c r="DP10">
+        <v>0.67978144173007204</v>
+      </c>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.97455656999999996</v>
       </c>
@@ -12253,8 +12356,11 @@
       <c r="DI11">
         <v>0.68045828692341703</v>
       </c>
+      <c r="DP11">
+        <v>0.84573378741811001</v>
+      </c>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.97525066000000005</v>
       </c>
@@ -12351,8 +12457,11 @@
       <c r="DI12">
         <v>0.52649089514327296</v>
       </c>
+      <c r="DP12">
+        <v>0.89342484847572301</v>
+      </c>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.97576589999999996</v>
       </c>
@@ -12453,8 +12562,11 @@
       <c r="DI13">
         <v>0.68749303042966503</v>
       </c>
+      <c r="DP13">
+        <v>0.61297637562980301</v>
+      </c>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.97638970000000003</v>
       </c>
@@ -12551,8 +12663,11 @@
       <c r="DI14">
         <v>0.54496903256558304</v>
       </c>
+      <c r="DP14">
+        <v>0.24174441492538401</v>
+      </c>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.97705995999999995</v>
       </c>
@@ -12643,8 +12758,11 @@
       <c r="CU15">
         <v>0.79071226818406803</v>
       </c>
+      <c r="DP15">
+        <v>0.81544948705027698</v>
+      </c>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:132" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.97779329999999998</v>
       </c>
@@ -12734,6 +12852,9 @@
       </c>
       <c r="CU16">
         <v>0.74189600318848503</v>
+      </c>
+      <c r="DP16">
+        <v>0.50660840116143402</v>
       </c>
     </row>
     <row r="17" spans="1:86" x14ac:dyDescent="0.2">

</xml_diff>